<commit_message>
revised PM calculation code
</commit_message>
<xml_diff>
--- a/data/emission calculations accra/traffic emissions calculations accra.xlsx
+++ b/data/emission calculations accra/traffic emissions calculations accra.xlsx
@@ -518,7 +518,8 @@
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -592,24 +593,24 @@
         <v>0.22800000000000001</v>
       </c>
       <c r="F9">
-        <f>E9*D9</f>
-        <v>21788.860143874739</v>
+        <f>E9*D9*10000</f>
+        <v>217888601.43874741</v>
       </c>
       <c r="G9" s="2">
         <f>F9/SUM(F$9:F$18)</f>
-        <v>0.14203152204748859</v>
+        <v>6.7405968772800112E-2</v>
       </c>
       <c r="H9" s="1">
         <f>F9*C24/B24</f>
-        <v>29791.908416981216</v>
+        <v>297919084.16981214</v>
       </c>
       <c r="I9" s="1">
         <f>F9*D24/B24</f>
-        <v>20354.052992868335</v>
+        <v>203540529.92868334</v>
       </c>
       <c r="J9" s="1">
         <f>F9*E24/B24</f>
-        <v>11351.143334088705</v>
+        <v>113511433.34088707</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -631,24 +632,24 @@
         <v>0.27600000000000002</v>
       </c>
       <c r="F10">
-        <f>E10*D10</f>
-        <v>3458.0168346735645</v>
+        <f>E10*D10*15000</f>
+        <v>51870252.520103469</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" ref="G10:G16" si="1">F10/SUM(F$9:F$18)</f>
-        <v>2.2541215605195203E-2</v>
+        <v>1.604656966229711E-2</v>
       </c>
       <c r="H10" s="1">
         <f>F10*C24/B24</f>
-        <v>4728.1464088857001</v>
+        <v>70922196.133285493</v>
       </c>
       <c r="I10" s="1">
         <f>F10*D24/B24</f>
-        <v>3230.3047262875293</v>
+        <v>48454570.894312941</v>
       </c>
       <c r="J10" s="1">
         <f>F10*E24/B24</f>
-        <v>1801.4914264850133</v>
+        <v>27022371.397275198</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -670,24 +671,24 @@
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="F11">
-        <f t="shared" ref="F11:F16" si="2">E11*D11</f>
-        <v>3364.5779480573929</v>
+        <f>E11*D11*10000</f>
+        <v>33645779.48057393</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="1"/>
-        <v>2.1932130632558468E-2</v>
+        <v>1.0408650778556867E-2</v>
       </c>
       <c r="H11" s="1">
         <f>F11</f>
-        <v>3364.5779480573929</v>
+        <v>33645779.48057393</v>
       </c>
       <c r="I11" s="1">
         <f>F11</f>
-        <v>3364.5779480573929</v>
+        <v>33645779.48057393</v>
       </c>
       <c r="J11" s="1">
         <f>F11</f>
-        <v>3364.5779480573929</v>
+        <v>33645779.48057393</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -709,24 +710,24 @@
         <v>0.27600000000000002</v>
       </c>
       <c r="F12">
-        <f>E12*D12</f>
-        <v>628.22792419101938</v>
+        <f>E12*D12*20000</f>
+        <v>12564558.483820388</v>
       </c>
       <c r="G12" s="2">
         <f t="shared" si="1"/>
-        <v>4.0951278624214073E-3</v>
+        <v>3.8869689887954268E-3</v>
       </c>
       <c r="H12" s="1">
         <f>F12*C26/B26</f>
-        <v>628.22792419101938</v>
+        <v>12564558.483820388</v>
       </c>
       <c r="I12" s="1">
         <f>F12*D26/B26</f>
-        <v>564.58885872316114</v>
+        <v>11291777.174463224</v>
       </c>
       <c r="J12" s="1">
         <f>F12*E26/B26</f>
-        <v>405.26445253997184</v>
+        <v>8105289.0507994378</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -748,24 +749,24 @@
         <v>6.9</v>
       </c>
       <c r="F13">
-        <f t="shared" si="2"/>
-        <v>17819.999096998734</v>
+        <f>E13*D13*150*365</f>
+        <v>975644950.56068063</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" si="1"/>
-        <v>0.11616034881673766</v>
+        <v>0.30182530263897683</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" ref="H13:H16" si="3">F13</f>
-        <v>17819.999096998734</v>
+        <f t="shared" ref="H13:H16" si="2">F13</f>
+        <v>975644950.56068063</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" ref="I13:I16" si="4">F13</f>
-        <v>17819.999096998734</v>
+        <f t="shared" ref="I13:I16" si="3">F13</f>
+        <v>975644950.56068063</v>
       </c>
       <c r="J13" s="1">
         <f>F13*E22/B22</f>
-        <v>23817.814051643265</v>
+        <v>1304025319.3274689</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -780,31 +781,31 @@
         <v>1.8411098512277145E-2</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" ref="D14:D16" si="5">B14/10</f>
+        <f t="shared" ref="D14:D16" si="4">B14/10</f>
         <v>5891.5515239286869</v>
       </c>
       <c r="E14">
         <v>7.9</v>
       </c>
       <c r="F14">
-        <f t="shared" si="2"/>
-        <v>46543.257039036631</v>
+        <f>E14*D14*25*2*365</f>
+        <v>849414440.96241844</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="1"/>
-        <v>0.30339400935391414</v>
+        <v>0.26277466055870696</v>
       </c>
       <c r="H14" s="1">
+        <f t="shared" si="2"/>
+        <v>849414440.96241844</v>
+      </c>
+      <c r="I14" s="1">
         <f t="shared" si="3"/>
-        <v>46543.257039036631</v>
-      </c>
-      <c r="I14" s="1">
-        <f t="shared" si="4"/>
-        <v>46543.257039036631</v>
+        <v>849414440.96241844</v>
       </c>
       <c r="J14" s="1">
         <f>F14</f>
-        <v>46543.257039036631</v>
+        <v>849414440.96241844</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -819,31 +820,31 @@
         <v>4.206690851288241E-2</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>13461.410724122372</v>
       </c>
       <c r="E15">
         <v>4.0890000000000004</v>
       </c>
       <c r="F15">
-        <f t="shared" si="2"/>
-        <v>55043.708450936385</v>
+        <f>E15*D15*25*2*365</f>
+        <v>1004547679.2295891</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="1"/>
-        <v>0.35880452849767253</v>
+        <v>0.31076664428439027</v>
       </c>
       <c r="H15" s="1">
+        <f t="shared" si="2"/>
+        <v>1004547679.2295891</v>
+      </c>
+      <c r="I15" s="1">
         <f t="shared" si="3"/>
-        <v>55043.708450936385</v>
-      </c>
-      <c r="I15" s="1">
-        <f t="shared" si="4"/>
-        <v>55043.708450936385</v>
+        <v>1004547679.2295891</v>
       </c>
       <c r="J15" s="1">
-        <f t="shared" ref="J15:J16" si="6">F15</f>
-        <v>55043.708450936385</v>
+        <f t="shared" ref="J15:J16" si="5">F15</f>
+        <v>1004547679.2295891</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -858,31 +859,31 @@
         <v>1.8196590803702265E-3</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>582.29090571847246</v>
       </c>
       <c r="E16">
         <v>8.1780000000000008</v>
       </c>
       <c r="F16">
-        <f t="shared" si="2"/>
-        <v>4761.9750269656679</v>
+        <f>E16*D16*25*2*365</f>
+        <v>86906044.24212344</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="1"/>
-        <v>3.1041117184012E-2</v>
+        <v>2.688523431547633E-2</v>
       </c>
       <c r="H16" s="1">
+        <f t="shared" si="2"/>
+        <v>86906044.24212344</v>
+      </c>
+      <c r="I16" s="1">
         <f t="shared" si="3"/>
-        <v>4761.9750269656679</v>
-      </c>
-      <c r="I16" s="1">
-        <f t="shared" si="4"/>
-        <v>4761.9750269656679</v>
+        <v>86906044.24212344</v>
       </c>
       <c r="J16" s="1">
-        <f t="shared" si="6"/>
-        <v>4761.9750269656679</v>
+        <f t="shared" si="5"/>
+        <v>86906044.24212344</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>